<commit_message>
first draft of data set
</commit_message>
<xml_diff>
--- a/SampleDataset.xlsx
+++ b/SampleDataset.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\github-sap\i313873\codeathon2018\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24540" windowHeight="11025"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
   <si>
     <t>AvgBackgroundQ</t>
   </si>
@@ -33,9 +29,6 @@
     <t>NodeId</t>
   </si>
   <si>
-    <t>FailedPostOutput</t>
-  </si>
-  <si>
     <t>ProductRelease</t>
   </si>
   <si>
@@ -48,36 +41,32 @@
     <t>CatalogSearchTime</t>
   </si>
   <si>
-    <t>NetworkConnectivity</t>
+    <t>NetworkConnectivitySNV-US1</t>
   </si>
   <si>
     <t>LogSizeVolumePercent</t>
-  </si>
-  <si>
-    <t>TimeSinceSystemIsUp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -92,43 +81,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -416,30 +388,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.85546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -470,14 +432,8 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>